<commit_message>
add screenshot picture and modify README.md to display them
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\fpgaProjects\soft_core_cpu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\fpgaProjects\soft_core_cpu\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5E93D3-C4CC-4A78-A7D7-8E3025C02234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8212F4-5ABA-4301-A14B-777716276C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="159">
   <si>
     <t>comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -663,6 +663,10 @@
   </si>
   <si>
     <t>check if condition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># of cycles</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -849,7 +853,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -904,20 +908,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1240,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC2C441-DEC2-4001-8CD5-3DBF91AD2891}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.7"/>
@@ -1252,12 +1265,13 @@
     <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.37890625" customWidth="1"/>
     <col min="7" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.37890625" customWidth="1"/>
-    <col min="11" max="11" width="63.09375" customWidth="1"/>
-    <col min="12" max="12" width="105.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.046875" customWidth="1"/>
+    <col min="11" max="11" width="64.1875" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="107.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
@@ -1292,10 +1306,13 @@
         <v>79</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1329,11 +1346,14 @@
       <c r="K2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="23">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
@@ -1367,11 +1387,14 @@
       <c r="K3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="23">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1405,11 +1428,14 @@
       <c r="K4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="23">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -1443,11 +1469,14 @@
       <c r="K5" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="23">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -1481,11 +1510,14 @@
       <c r="K6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="23">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1519,11 +1551,14 @@
       <c r="K7" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="23">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1557,11 +1592,14 @@
       <c r="K8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="23">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -1595,11 +1633,14 @@
       <c r="K9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="23">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A10" s="4" t="s">
         <v>115</v>
       </c>
@@ -1633,11 +1674,14 @@
       <c r="K10" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="23">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A11" s="4" t="s">
         <v>111</v>
       </c>
@@ -1671,11 +1715,14 @@
       <c r="K11" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="23">
+        <v>1</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1709,11 +1756,14 @@
       <c r="K12" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="23">
+        <v>2</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
@@ -1747,11 +1797,14 @@
       <c r="K13" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="23">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
@@ -1785,11 +1838,14 @@
       <c r="K14" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="23">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A15" s="4" t="s">
         <v>113</v>
       </c>
@@ -1823,11 +1879,14 @@
       <c r="K15" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="23">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -1861,11 +1920,14 @@
       <c r="K16" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="23">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
@@ -1899,11 +1961,14 @@
       <c r="K17" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="23">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
@@ -1937,11 +2002,14 @@
       <c r="K18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="23">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A19" s="4" t="s">
         <v>68</v>
       </c>
@@ -1975,11 +2043,14 @@
       <c r="K19" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="23">
+        <v>1</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A22" s="15" t="s">
         <v>61</v>
       </c>
@@ -1992,8 +2063,9 @@
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
       <c r="J22" s="17"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.7">
+      <c r="L22" s="24"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -2008,8 +2080,9 @@
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.7">
+      <c r="L23" s="25"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -2024,8 +2097,9 @@
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.7">
+      <c r="L24" s="25"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -2040,8 +2114,9 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.7">
+      <c r="L25" s="25"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A26" s="2">
         <v>4</v>
       </c>
@@ -2056,6 +2131,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
+      <c r="L26" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2074,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DC6A67-9716-471F-B242-870F8D2F0ED7}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.7"/>
@@ -2125,7 +2201,7 @@
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="21" t="s">
         <v>96</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2134,30 +2210,30 @@
       <c r="C4" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="20"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A5" s="18"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="12" t="s">
         <v>106</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A6" s="18"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="21" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -2166,173 +2242,173 @@
       <c r="C7" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="18" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A8" s="18"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="21"/>
+      <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A9" s="18"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="12" t="s">
         <v>120</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A10" s="18"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="12" t="s">
         <v>100</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A11" s="18"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="12" t="s">
         <v>123</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="19"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A12" s="18"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="21"/>
+      <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A13" s="18"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="19"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="12" t="s">
         <v>147</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A15" s="18"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A16" s="18"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A17" s="18"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="12" t="s">
         <v>145</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="19"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A18" s="18"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="12" t="s">
         <v>149</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="19"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A19" s="18"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="12" t="s">
         <v>151</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="19"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A20" s="18"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D20" s="21"/>
+      <c r="D20" s="19"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A21" s="18"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="12" t="s">
         <v>152</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D21" s="21"/>
+      <c r="D21" s="19"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A22" s="18"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="20"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="21" t="s">
         <v>116</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>100</v>
       </c>
       <c r="C23" s="11"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A24" s="18"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="12" t="s">
         <v>117</v>
       </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="22"/>
+      <c r="D24" s="20"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A25" s="10" t="s">
@@ -2345,7 +2421,7 @@
       <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="21" t="s">
         <v>126</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -2354,87 +2430,87 @@
       <c r="C26" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="20"/>
+      <c r="D26" s="18"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A27" s="18"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="12" t="s">
         <v>138</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="21"/>
+      <c r="D27" s="19"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A28" s="18"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="12" t="s">
         <v>137</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="21"/>
+      <c r="D28" s="19"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A29" s="18"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="21"/>
+      <c r="D29" s="19"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A30" s="18"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="21"/>
+      <c r="D30" s="19"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A31" s="18"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="12" t="s">
         <v>132</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="21"/>
+      <c r="D31" s="19"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A32" s="18"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="21"/>
+      <c r="D32" s="19"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A33" s="18"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="12" t="s">
         <v>134</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="21"/>
+      <c r="D33" s="19"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A34" s="18"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="12" t="s">
         <v>121</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
more impelmentation and piplined schematic draw io picture
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\fpgaProjects\soft_core_cpu\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\coding\softcore_cpu\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8212F4-5ABA-4301-A14B-777716276C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA8290-2D2E-4AEE-9562-9F4DC6898A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
@@ -254,10 +254,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bgt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">branch greater than </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -330,10 +326,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jump to PC + 2 if value stored in reg_a is greater than value in accumulator, else go to PC + 1 which is the default next instruction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>jump to PC + 2 if value stored in reg_a is equal to value in reg_acc, else go to PC + 1 which is the default next instruction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -402,10 +394,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PC = reg_a &gt; reg_acc ? PC + 2 : PC + 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PC = reg_a == reg_acc ? PC + 2 : PC + 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -666,26 +654,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t># of cycles</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>bge</t>
+  </si>
+  <si>
+    <t>PC = reg_a &gt; = reg_acc ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>jump to PC + 2 if value stored in reg_a is greater or equal to the value in accumulator, else go to PC + 1 which is the default next instruction</t>
+  </si>
+  <si>
+    <t># of cycles in single cycle memory design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -694,7 +690,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -897,6 +893,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,15 +927,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,25 +1251,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC2C441-DEC2-4001-8CD5-3DBF91AD2891}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.76171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.37890625" customWidth="1"/>
-    <col min="7" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.046875" customWidth="1"/>
-    <col min="11" max="11" width="64.1875" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="107.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="64.21875" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="124.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -1288,7 +1284,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>47</v>
@@ -1303,7 +1299,7 @@
         <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>158</v>
@@ -1312,7 +1308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1344,16 +1340,16 @@
         <v>16</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" s="23">
+        <v>74</v>
+      </c>
+      <c r="L2" s="14">
         <v>1</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
@@ -1382,19 +1378,19 @@
         <v>46</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="23">
+        <v>75</v>
+      </c>
+      <c r="L3" s="14">
         <v>1</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1426,16 +1422,16 @@
         <v>17</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" s="23">
+        <v>78</v>
+      </c>
+      <c r="L4" s="14">
         <v>1</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -1464,19 +1460,19 @@
         <v>46</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" s="23">
+        <v>79</v>
+      </c>
+      <c r="L5" s="14">
         <v>1</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
@@ -1508,16 +1504,16 @@
         <v>19</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" s="23">
+        <v>80</v>
+      </c>
+      <c r="L6" s="14">
         <v>1</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:13">
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
@@ -1549,16 +1545,16 @@
         <v>18</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" s="23">
+        <v>81</v>
+      </c>
+      <c r="L7" s="14">
         <v>1</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1590,16 +1586,16 @@
         <v>20</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L8" s="23">
+        <v>83</v>
+      </c>
+      <c r="L8" s="14">
         <v>1</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -1631,18 +1627,18 @@
         <v>21</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L9" s="23">
+        <v>82</v>
+      </c>
+      <c r="L9" s="14">
         <v>1</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
@@ -1669,21 +1665,21 @@
         <v>41</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L10" s="23">
+        <v>84</v>
+      </c>
+      <c r="L10" s="14">
         <v>1</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
@@ -1710,19 +1706,19 @@
         <v>41</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L11" s="23">
+        <v>105</v>
+      </c>
+      <c r="L11" s="14">
         <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.7">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1754,16 +1750,16 @@
         <v>50</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="L12" s="23">
+        <v>85</v>
+      </c>
+      <c r="L12" s="14">
         <v>2</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
@@ -1795,16 +1791,16 @@
         <v>51</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="L13" s="23">
+        <v>86</v>
+      </c>
+      <c r="L13" s="14">
         <v>2</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
@@ -1836,18 +1832,18 @@
         <v>52</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="L14" s="23">
+        <v>87</v>
+      </c>
+      <c r="L14" s="14">
         <v>1</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B15" s="13">
         <v>1</v>
@@ -1874,19 +1870,19 @@
         <v>46</v>
       </c>
       <c r="J15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L15" s="14">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="L15" s="23">
-        <v>2</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.7">
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -1918,18 +1914,18 @@
         <v>53</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L16" s="23">
+        <v>89</v>
+      </c>
+      <c r="L16" s="14">
         <v>1</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="4" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="B17" s="13">
         <v>1</v>
@@ -1956,19 +1952,19 @@
         <v>41</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="L17" s="23">
+        <v>156</v>
+      </c>
+      <c r="L17" s="14">
         <v>1</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.7">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
@@ -2000,18 +1996,18 @@
         <v>54</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="L18" s="23">
+        <v>90</v>
+      </c>
+      <c r="L18" s="14">
         <v>1</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
@@ -2038,100 +2034,100 @@
         <v>41</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="L19" s="23">
+        <v>91</v>
+      </c>
+      <c r="L19" s="14">
         <v>1</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A22" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="L22" s="15"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="17"/>
-      <c r="L22" s="24"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="L23" s="25"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="L23" s="16"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="2">
         <v>2</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="L24" s="25"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="B24" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="L24" s="16"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="2">
         <v>3</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="L25" s="25"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="B25" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="L25" s="16"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="2">
         <v>4</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="L26" s="25"/>
+      <c r="B26" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="L26" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2151,18 +2147,18 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.1875" customWidth="1"/>
-    <col min="3" max="3" width="73.90234375" customWidth="1"/>
-    <col min="4" max="4" width="33.6171875" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="73.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>22</v>
       </c>
@@ -2176,341 +2172,341 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2" s="11"/>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:4" ht="43.2">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="24"/>
+      <c r="B5" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="24"/>
+      <c r="B6" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A4" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A5" s="21"/>
-      <c r="B5" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A6" s="21"/>
-      <c r="B6" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="B7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A7" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="24"/>
+      <c r="B8" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="24"/>
+      <c r="B9" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="24"/>
+      <c r="B10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="22"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="24"/>
+      <c r="B11" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="22"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="24"/>
+      <c r="B12" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="24"/>
+      <c r="B13" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="22"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="24"/>
+      <c r="B14" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="24"/>
+      <c r="B15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="24"/>
+      <c r="B16" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="24"/>
+      <c r="B17" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="24"/>
+      <c r="B18" s="12" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A8" s="21"/>
-      <c r="B8" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A9" s="21"/>
-      <c r="B9" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A10" s="21"/>
-      <c r="B10" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A11" s="21"/>
-      <c r="B11" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="19"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A12" s="21"/>
-      <c r="B12" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" s="19"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A13" s="21"/>
-      <c r="B13" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="19"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A14" s="21"/>
-      <c r="B14" s="12" t="s">
+      <c r="C18" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="24"/>
+      <c r="B19" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="19"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A15" s="21"/>
-      <c r="B15" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="19"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A16" s="21"/>
-      <c r="B16" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A17" s="21"/>
-      <c r="B17" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A18" s="21"/>
-      <c r="B18" s="12" t="s">
+      <c r="D19" s="22"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="24"/>
+      <c r="B20" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="24"/>
+      <c r="B21" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D18" s="19"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A19" s="21"/>
-      <c r="B19" s="12" t="s">
+      <c r="C21" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A20" s="21"/>
-      <c r="B20" s="12" t="s">
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="24"/>
+      <c r="B22" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="23"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="19"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A21" s="21"/>
-      <c r="B21" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A22" s="21"/>
-      <c r="B22" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="20"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A23" s="21" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="24"/>
+      <c r="B24" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="23"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="18"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A24" s="21"/>
-      <c r="B24" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="20"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A25" s="10" t="s">
-        <v>119</v>
-      </c>
       <c r="B25" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A26" s="21" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="24"/>
+      <c r="B27" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="24"/>
+      <c r="B28" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="24"/>
+      <c r="B29" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" s="18"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A27" s="21"/>
-      <c r="B27" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C27" s="11" t="s">
+      <c r="D29" s="22"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="24"/>
+      <c r="B30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="24"/>
+      <c r="B31" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="19"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A28" s="21"/>
-      <c r="B28" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="19"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A29" s="21"/>
-      <c r="B29" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="11" t="s">
+      <c r="C31" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="22"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="24"/>
+      <c r="B32" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="19"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A30" s="21"/>
-      <c r="B30" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C30" s="11" t="s">
+      <c r="D32" s="22"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="24"/>
+      <c r="B33" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="19"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A31" s="21"/>
-      <c r="B31" s="12" t="s">
+      <c r="C33" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" s="19"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A32" s="21"/>
-      <c r="B32" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C32" s="11" t="s">
+      <c r="D33" s="22"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="24"/>
+      <c r="B34" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D32" s="19"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A33" s="21"/>
-      <c r="B33" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D33" s="19"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.7">
-      <c r="A34" s="21"/>
-      <c r="B34" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="20"/>
+      <c r="D34" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
hardcode comparator input to reg_acc and reg_b, and some more drawing, as well as implement branch decision module and some of control module
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\coding\softcore_cpu\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FA8290-2D2E-4AEE-9562-9F4DC6898A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7150397-02BF-47EF-A20F-89021E5AE272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
@@ -37,22 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="157">
   <si>
     <t>comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>reg_a[2]</t>
-  </si>
-  <si>
-    <t>reg_a[1]</t>
-  </si>
-  <si>
-    <t>reg_a[1]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>op_code[0]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -69,601 +59,572 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bitwise AND operation between reg_a and reg_acc, then store in reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bitwise OR operation between reg_a and reg_acc, then store in reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bitwise XOR operation between reg_a and reg_acc, then store in reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imm[3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>register add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>register shift</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary and</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unary not</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary or</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary xor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISA implementation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set reg_acc to 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shift by an immidiate value, immidiate value is in 2s complement. Immidiate value = -8 ~ 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>not</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>and</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>or</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jmpadr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imm[2]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imm[1]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imm[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[2]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bit[1]</t>
+  </si>
+  <si>
+    <t>bit[0]</t>
+  </si>
+  <si>
+    <t>load byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>store byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jump address</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch less than</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch equal to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">branch greater than </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add immidiate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shift immidiate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all immidiate values and values stored in registers are in 2s complement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unconditionally jump to a specific address in memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bneq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch not equal to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jump immidiate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unconditionally jump to a specific offset relative to program counter in memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>utility bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>utility bit is used for different things based on different instructions. See table above. This is used so immidiate value can have a larger range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In presudo verilog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC = PC + imm[3:0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instruction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>store value in register 3'b101 to adderss 8'b10101010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addi 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add 0 to accumulator register equals to doing nothing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>neg 8 causes shifter to underflow which means we lose all the bits in reg_acc, which also means we just set all bits to zero. This is better than addi 0 to a random register then ldacc into the accumulator register, which takes 2 instructions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sh -8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set accumulator register to 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>put 8'b10101010 into accumulator register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ld 101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>store value into memory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>for loop that runs 3 times</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addi 10101010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set 0 to accumulator register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copy accumulator register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpypc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpy program counter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jmpi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copy register R[101] to accumulator register (R[111])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add 101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpy 101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copy accumulator register R[111] to register R[101]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpy 001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addi 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">set 3 to accumulator register </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpy 000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set R[000] to 0, R[000] will be our counter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set R[001] to be 3. R[001] will be our upper bound</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jump by 8 instructions if R[101] == R[111]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beq 101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>else</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>else case starts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>else case ends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jumpi 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if true case starts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addi 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if true case ends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>after if statement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jumpi 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jumpi 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jump to after if statement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">sh -8 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copy R[010] to accumulator register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add 010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code inside of for loop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add 000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>for (int I = 0;i&lt;3;i++) {R[010] += 9}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addi 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>increment counter by 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beq 001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if counter is not 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jump -7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">addi 0 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if counter is 3, continue program execution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>program execution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check counter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copy counter to accumulator register</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check if condition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bge</t>
+  </si>
+  <si>
+    <t># of cycles in single cycle memory design</t>
+  </si>
+  <si>
+    <t>reg_acc = reg_acc + reg_b</t>
+  </si>
+  <si>
+    <t>reg_acc = reg_b &gt; 0 ? reg_acc &lt;&lt; reg_b : reg_acc &gt;&gt; (~reg_b + 1)</t>
+  </si>
+  <si>
+    <t>reg_b[2]</t>
+  </si>
+  <si>
+    <t>reg_b[1]</t>
+  </si>
+  <si>
+    <t>reg_b[0]</t>
+  </si>
+  <si>
+    <t>reg_b = PC</t>
+  </si>
+  <si>
+    <t>copy current instruction address in PC into reg_b</t>
+  </si>
+  <si>
+    <t>PC = reg_b</t>
+  </si>
+  <si>
+    <t>reg_b can of the 8 general purpose registers synthesized, including R[111] which is the accumulator register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add value in reg_b to value in reg_acc, then store in reg_acc. </t>
+  </si>
+  <si>
+    <t>reg_acc = reg_acc + imm[3:0]</t>
+  </si>
+  <si>
+    <t>add value in reg_acc with value in reg_b, then store in reg_acc. Immidiate value = -8 ~ 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift value in reg_acc by value in reg_b, then store in reg_acc. </t>
+  </si>
+  <si>
+    <t>reg_acc = imm[3:0] &gt; 0 ? reg_acc &lt;&lt; imm[3:0] : reg_acc &gt;&gt; (~imm[3:0] + 1)</t>
+  </si>
+  <si>
+    <t>reg_acc = ~reg_acc</t>
   </si>
   <si>
     <t>unary NOT operation on reg_acc, then store in reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>no operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imm[3]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>register add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>register shift</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>binary and</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unary not</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>binary or</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>binary xor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>operation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISA implementation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set reg_acc to 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add value in reg_acc with value in reg_a, then store in reg_acc. Immidiate value = -8 ~ 7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shift by an immidiate value, immidiate value is in 2s complement. Immidiate value = -8 ~ 7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>not</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>and</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>or</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jmpadr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>blt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>beq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_a[0]</t>
-  </si>
-  <si>
-    <t>reg_a[0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imm[2]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imm[1]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imm[0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bit[2]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bit[1]</t>
-  </si>
-  <si>
-    <t>bit[0]</t>
-  </si>
-  <si>
-    <t>load byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>store byte</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jump address</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branch less than</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branch equal to</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">branch greater than </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add immidiate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shift immidiate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">add value in reg_a to value in reg_acc, then store in reg_acc. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">shift value in reg_acc by value in reg_a, then store in reg_acc. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Note</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>all immidiate values and values stored in registers are in 2s complement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg_acc = reg_acc &amp; reg_b</t>
+  </si>
+  <si>
+    <t>bitwise AND operation between reg_b and reg_acc, then store in reg_acc</t>
+  </si>
+  <si>
+    <t>reg_acc = reg_acc | reg_b</t>
+  </si>
+  <si>
+    <t>bitwise OR operation between reg_b and reg_acc, then store in reg_acc</t>
+  </si>
+  <si>
+    <t>reg_acc = reg_acc ^ reg_b</t>
+  </si>
+  <si>
+    <t>bitwise XOR operation between reg_b and reg_acc, then store in reg_acc</t>
+  </si>
+  <si>
+    <t>reg_b = reg_acc</t>
+  </si>
+  <si>
+    <t>copy value in reg_acc into reg_b</t>
+  </si>
+  <si>
+    <t>reg_b = M[reg_acc]</t>
+  </si>
+  <si>
+    <t>load 1 byte from address B in memory, then store the value in reg_b. B is the value in reg_acc</t>
+  </si>
+  <si>
+    <t>M[reg_acc] = reg_b</t>
+  </si>
+  <si>
+    <t>store value in reg_b to address B in memory. B is the value in reg_acc</t>
+  </si>
+  <si>
+    <t>PC = reg_b &lt; reg_acc ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>PC = reg_b &gt; = reg_acc ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>PC = reg_b == reg_acc ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>PC = reg_b != reg_acc ? PC + 2 : PC + 1</t>
   </si>
   <si>
     <t>reg_acc is the special accumulator register which input is the result of the ALU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy value in reg_acc into reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>load 1 byte from address B in memory, then store the value in reg_a. B is the value in reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>store value in reg_a to address B in memory. B is the value in reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unconditionally jump to a specific address in memory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bneq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>branch not equal to</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jump immidiate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unconditionally jump to a specific offset relative to program counter in memory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>utility bit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jump to PC + 2 if value stored in reg_a is less than value in accumulator, else go to PC + 1 which is the default next instruction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jump to PC + 2 if value stored in reg_a is equal to value in reg_acc, else go to PC + 1 which is the default next instruction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = reg_acc + reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = reg_acc + imm[3:0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>utility bit is used for different things based on different instructions. See table above. This is used so immidiate value can have a larger range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In presudo verilog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = reg_a &gt; 0 ? reg_acc &lt;&lt; reg_a : reg_acc &gt;&gt; (~reg_a + 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = imm[3:0] &gt; 0 ? reg_acc &lt;&lt; imm[3:0] : reg_acc &gt;&gt; (~imm[3:0] + 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = ~reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = reg_acc &amp; reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = reg_acc ^ reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_acc = reg_acc | reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_a = reg_acc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_a = M[reg_acc]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M[reg_acc] = reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC = reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC = PC + imm[3:0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC = reg_a &lt; reg_acc ? PC + 2 : PC + 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC = reg_a == reg_acc ? PC + 2 : PC + 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC = reg_a != reg_acc ? PC + 2 : PC + 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>instruction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>store value in register 3'b101 to adderss 8'b10101010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addi 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add 0 to accumulator register equals to doing nothing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>neg 8 causes shifter to underflow which means we lose all the bits in reg_acc, which also means we just set all bits to zero. This is better than addi 0 to a random register then ldacc into the accumulator register, which takes 2 instructions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sh -8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set accumulator register to 0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>put 8'b10101010 into accumulator register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ld 101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>store value into memory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>for loop that runs 3 times</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addi 10101010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set 0 to accumulator register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_a = PC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy accumulator register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy current instruction address in PC into reg_a</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpypc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpy program counter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jmpi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reg_a can of the 8 general purpose registers synthesized, including R[111] which is the accumulator register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy register R[101] to accumulator register (R[111])</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add 101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpy 101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy accumulator register R[111] to register R[101]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpy 001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addi 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">set 3 to accumulator register </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpy 000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set R[000] to 0, R[000] will be our counter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>set R[001] to be 3. R[001] will be our upper bound</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jump by 8 instructions if R[101] == R[111]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>beq 101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if true</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>else</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>else case starts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>else case ends</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jumpi 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if true case starts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addi 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if true case ends</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>after if statement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jumpi 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jumpi 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jump to after if statement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">sh -8 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy R[010] to accumulator register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add 010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>code inside of for loop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add 000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>for (int I = 0;i&lt;3;i++) {R[010] += 9}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>addi 9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>increment counter by 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>beq 001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if counter is not 3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jump -7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">addi 0 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if counter is 3, continue program execution</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>program execution</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>check counter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>copy counter to accumulator register</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>check if condition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bge</t>
-  </si>
-  <si>
-    <t>PC = reg_a &gt; = reg_acc ? PC + 2 : PC + 1</t>
-  </si>
-  <si>
-    <t>jump to PC + 2 if value stored in reg_a is greater or equal to the value in accumulator, else go to PC + 1 which is the default next instruction</t>
-  </si>
-  <si>
-    <t># of cycles in single cycle memory design</t>
+  </si>
+  <si>
+    <t>jump to PC + 2 if value stored in reg_b is less than value in accumulator, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
+  </si>
+  <si>
+    <t>jump to PC + 2 if value stored in reg_b is greater or equal to the value in accumulator, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
+  </si>
+  <si>
+    <t>jump to PC + 2 if value stored in reg_b is equal to value in reg_acc, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC2C441-DEC2-4001-8CD5-3DBF91AD2891}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1261,56 +1222,56 @@
     <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
     <col min="11" max="11" width="64.21875" customWidth="1"/>
     <col min="12" max="12" width="11.109375" customWidth="1"/>
-    <col min="13" max="13" width="124.109375" customWidth="1"/>
+    <col min="13" max="13" width="132.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B2" s="13">
         <v>0</v>
@@ -1325,33 +1286,33 @@
         <v>0</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="L2" s="14">
         <v>1</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B3" s="13">
         <v>0</v>
@@ -1366,33 +1327,33 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="L3" s="14">
         <v>1</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>25</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B4" s="13">
         <v>0</v>
@@ -1407,33 +1368,33 @@
         <v>0</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="L4" s="14">
         <v>1</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B5" s="13">
         <v>0</v>
@@ -1448,33 +1409,33 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="L5" s="14">
         <v>1</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
@@ -1489,33 +1450,33 @@
         <v>0</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
       <c r="L6" s="14">
         <v>1</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -1530,33 +1491,33 @@
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="L7" s="14">
         <v>1</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>8</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B8" s="13">
         <v>0</v>
@@ -1571,74 +1532,74 @@
         <v>0</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>83</v>
+        <v>139</v>
       </c>
       <c r="L8" s="14">
         <v>1</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>9</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="13">
-        <v>0</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="G9" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="L9" s="14">
         <v>1</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>10</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
@@ -1656,30 +1617,30 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>84</v>
+        <v>143</v>
       </c>
       <c r="L10" s="14">
         <v>1</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
@@ -1697,30 +1658,30 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="L11" s="14">
         <v>1</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
@@ -1735,33 +1696,33 @@
         <v>1</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="L12" s="14">
         <v>2</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
@@ -1776,33 +1737,33 @@
         <v>0</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I13" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="K13" s="3" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="L13" s="14">
         <v>2</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>65</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
@@ -1817,33 +1778,33 @@
         <v>1</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="L14" s="14">
         <v>1</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B15" s="13">
         <v>1</v>
@@ -1858,33 +1819,33 @@
         <v>0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="L15" s="14">
         <v>2</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B16" s="13">
         <v>1</v>
@@ -1899,74 +1860,74 @@
         <v>1</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="K16" s="3" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="L16" s="14">
         <v>1</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>72</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="13">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="L17" s="14">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B17" s="13">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13">
-        <v>1</v>
-      </c>
-      <c r="D17" s="13">
-        <v>1</v>
-      </c>
-      <c r="E17" s="13">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="L17" s="14">
-        <v>1</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B18" s="13">
         <v>1</v>
@@ -1984,30 +1945,30 @@
         <v>0</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="L18" s="14">
         <v>1</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
@@ -2025,30 +1986,30 @@
         <v>1</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="L19" s="14">
         <v>1</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="18" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -2066,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -2083,7 +2044,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -2100,7 +2061,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -2117,7 +2078,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -2160,13 +2121,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>0</v>
@@ -2174,128 +2135,128 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="43.2">
       <c r="A3" s="10" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="24" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="24"/>
       <c r="B5" s="12" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="24"/>
       <c r="B6" s="12" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="24" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="24"/>
       <c r="B8" s="12" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="24"/>
       <c r="B9" s="12" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="24"/>
       <c r="B10" s="12" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="24"/>
       <c r="B11" s="12" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="24"/>
       <c r="B12" s="12" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="24"/>
       <c r="B13" s="12" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="22"/>
@@ -2303,27 +2264,27 @@
     <row r="14" spans="1:4">
       <c r="A14" s="24"/>
       <c r="B14" s="12" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="D14" s="22"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="24"/>
       <c r="B15" s="12" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="D15" s="22"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="24"/>
       <c r="B16" s="12" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="22"/>
@@ -2331,69 +2292,69 @@
     <row r="17" spans="1:4">
       <c r="A17" s="24"/>
       <c r="B17" s="12" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="24"/>
       <c r="B18" s="12" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="D18" s="22"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="24"/>
       <c r="B19" s="12" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="24"/>
       <c r="B20" s="12" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="D20" s="22"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="24"/>
       <c r="B21" s="12" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="D21" s="22"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="24"/>
       <c r="B22" s="12" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="D22" s="23"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="24" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="21"/>
@@ -2401,110 +2362,110 @@
     <row r="24" spans="1:4">
       <c r="A24" s="24"/>
       <c r="B24" s="12" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="23"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="10" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="24" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="24"/>
       <c r="B27" s="12" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="D27" s="22"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="24"/>
       <c r="B28" s="12" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="D28" s="22"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="24"/>
       <c r="B29" s="12" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="24"/>
       <c r="B30" s="12" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="D30" s="22"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="24"/>
       <c r="B31" s="12" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="D31" s="22"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="24"/>
       <c r="B32" s="12" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="D32" s="22"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="24"/>
       <c r="B33" s="12" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="D33" s="22"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="24"/>
       <c r="B34" s="12" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="D34" s="23"/>
     </row>

</xml_diff>

<commit_message>
compute control signals in isa.xlsx and add more drawing details
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\coding\softcore_cpu\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7150397-02BF-47EF-A20F-89021E5AE272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8A167C-0022-4291-BA55-3A8E5F661F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
   <sheets>
-    <sheet name="ISA" sheetId="1" r:id="rId1"/>
-    <sheet name="presudo instructions" sheetId="2" r:id="rId2"/>
+    <sheet name="control signal decode" sheetId="4" r:id="rId1"/>
+    <sheet name="ISA" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="presudo instructions" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="172">
   <si>
     <t>comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -603,35 +605,80 @@
     <t>store value in reg_b to address B in memory. B is the value in reg_acc</t>
   </si>
   <si>
-    <t>PC = reg_b &lt; reg_acc ? PC + 2 : PC + 1</t>
-  </si>
-  <si>
-    <t>PC = reg_b &gt; = reg_acc ? PC + 2 : PC + 1</t>
-  </si>
-  <si>
-    <t>PC = reg_b == reg_acc ? PC + 2 : PC + 1</t>
-  </si>
-  <si>
-    <t>PC = reg_b != reg_acc ? PC + 2 : PC + 1</t>
-  </si>
-  <si>
     <t>reg_acc is the special accumulator register which input is the result of the ALU</t>
   </si>
   <si>
-    <t>jump to PC + 2 if value stored in reg_b is less than value in accumulator, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
-  </si>
-  <si>
-    <t>jump to PC + 2 if value stored in reg_b is greater or equal to the value in accumulator, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
-  </si>
-  <si>
-    <t>jump to PC + 2 if value stored in reg_b is equal to value in reg_acc, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
+    <t>PC = reg_acc &lt; reg_b ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>PC = reg_acc &gt; = reg_b ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>PC = reg_acc == reg_b ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>PC = reg_acc != reg_b ? PC + 2 : PC + 1</t>
+  </si>
+  <si>
+    <t>jump to PC + 2 if value stored in reg_acc is equal to value in reg_b, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
+  </si>
+  <si>
+    <t>jump to PC + 2 if value stored in reg_acc is greater or equal to the value in reg_b, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
+  </si>
+  <si>
+    <t>jump to PC + 2 if value stored in reg_acc is less than value in reg_b, else go to PC + 1 which is the default next instruction. Note imm = 2</t>
+  </si>
+  <si>
+    <t>alu_mode</t>
+  </si>
+  <si>
+    <t>ALU_MODE_ADD</t>
+  </si>
+  <si>
+    <t>ALU_MODE_NOT</t>
+  </si>
+  <si>
+    <t>ALU_MODE_AND</t>
+  </si>
+  <si>
+    <t>ALU_MODE_OR</t>
+  </si>
+  <si>
+    <t>ALU_MODE_XOR</t>
+  </si>
+  <si>
+    <t>ALU_MODE_SHIFT</t>
+  </si>
+  <si>
+    <t>ALU_MODE_BYPASS_A</t>
+  </si>
+  <si>
+    <t>ALU_MODE_BYPASS_B</t>
+  </si>
+  <si>
+    <t>rf_write_en</t>
+  </si>
+  <si>
+    <t>alu_a_sel : reg_acc 0 / PC 1</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>alu_b_sel : reg_b 0 / imm 1</t>
+  </si>
+  <si>
+    <t>mem_write_sel : alu_out 0 / dmem_out 1</t>
+  </si>
+  <si>
+    <t>mem_write_en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,6 +701,14 @@
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -810,7 +865,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -889,6 +944,21 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,8 +967,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBF8CF8"/>
       <color rgb="FFFFFD97"/>
-      <color rgb="FFBF8CF8"/>
       <color rgb="FFFF9797"/>
     </mruColors>
   </colors>
@@ -1209,11 +1279,1148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B97F70D-B131-4050-83E1-4FBF1CD85DFC}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+    <col min="11" max="11" width="64.21875" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" customWidth="1"/>
+    <col min="15" max="15" width="25.44140625" customWidth="1"/>
+    <col min="16" max="16" width="38" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="P1" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M2" s="14">
+        <v>1</v>
+      </c>
+      <c r="N2" s="14">
+        <v>0</v>
+      </c>
+      <c r="O2" s="14">
+        <v>0</v>
+      </c>
+      <c r="P2" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M3" s="14">
+        <v>1</v>
+      </c>
+      <c r="N3" s="14">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14">
+        <v>1</v>
+      </c>
+      <c r="P3" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="M4" s="14">
+        <v>1</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="M5" s="14">
+        <v>1</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <v>1</v>
+      </c>
+      <c r="P5" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="M6" s="14">
+        <v>1</v>
+      </c>
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="P6" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="M7" s="14">
+        <v>1</v>
+      </c>
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0</v>
+      </c>
+      <c r="P7" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="M8" s="14">
+        <v>1</v>
+      </c>
+      <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0</v>
+      </c>
+      <c r="P8" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M9" s="14">
+        <v>1</v>
+      </c>
+      <c r="N9" s="14">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0</v>
+      </c>
+      <c r="P9" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M10" s="14">
+        <v>1</v>
+      </c>
+      <c r="N10" s="14">
+        <v>0</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="P10" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M11" s="14">
+        <v>1</v>
+      </c>
+      <c r="N11" s="14">
+        <v>1</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="P11" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M12" s="14">
+        <v>1</v>
+      </c>
+      <c r="N12" s="14">
+        <v>0</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="P12" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0</v>
+      </c>
+      <c r="N13" s="14">
+        <v>0</v>
+      </c>
+      <c r="O13" s="14">
+        <v>0</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
+      <c r="N15" s="14">
+        <v>1</v>
+      </c>
+      <c r="O15" s="14">
+        <v>1</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M16" s="14">
+        <v>0</v>
+      </c>
+      <c r="N16" s="14">
+        <v>1</v>
+      </c>
+      <c r="O16" s="14">
+        <v>1</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="13">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M17" s="14">
+        <v>0</v>
+      </c>
+      <c r="N17" s="14">
+        <v>1</v>
+      </c>
+      <c r="O17" s="14">
+        <v>1</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
+      <c r="N18" s="14">
+        <v>1</v>
+      </c>
+      <c r="O18" s="14">
+        <v>1</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13">
+        <v>1</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M19" s="14">
+        <v>0</v>
+      </c>
+      <c r="N19" s="14">
+        <v>1</v>
+      </c>
+      <c r="O19" s="14">
+        <v>1</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="28"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="L23" s="16"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="2">
+        <v>2</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="L24" s="16"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="2">
+        <v>3</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="L25" s="16"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="2">
+        <v>4</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="L26" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B26:J26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC2C441-DEC2-4001-8CD5-3DBF91AD2891}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K19" sqref="A1:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1875,13 +3082,13 @@
         <v>43</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L16" s="14">
         <v>1</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1916,7 +3123,7 @@
         <v>45</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L17" s="14">
         <v>1</v>
@@ -1957,13 +3164,13 @@
         <v>44</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L18" s="14">
         <v>1</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1998,13 +3205,13 @@
         <v>52</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L19" s="14">
         <v>1</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -2061,7 +3268,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -2103,7 +3310,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB60AA9-9903-422B-A5D3-D91275F59C34}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DC6A67-9716-471F-B242-870F8D2F0ED7}">
   <dimension ref="A1:D34"/>
   <sheetViews>

</xml_diff>

<commit_message>
finish implementing control signals and add memory modules.
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\coding\softcore_cpu\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8A167C-0022-4291-BA55-3A8E5F661F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF70284-F689-4E11-A676-AFB0380F758B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
   <sheets>
     <sheet name="control signal decode" sheetId="4" r:id="rId1"/>
     <sheet name="ISA" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
-    <sheet name="presudo instructions" sheetId="2" r:id="rId4"/>
+    <sheet name="presudo instructions" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -668,10 +667,10 @@
     <t>alu_b_sel : reg_b 0 / imm 1</t>
   </si>
   <si>
-    <t>mem_write_sel : alu_out 0 / dmem_out 1</t>
-  </si>
-  <si>
     <t>mem_write_en</t>
+  </si>
+  <si>
+    <t>rf_write_sel : alu_out 0 / dmem_out 1</t>
   </si>
 </sst>
 </file>
@@ -865,7 +864,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -917,8 +916,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -928,6 +933,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -943,21 +951,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1282,19 +1275,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B97F70D-B131-4050-83E1-4FBF1CD85DFC}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="26.33203125" customWidth="1"/>
     <col min="11" max="11" width="64.21875" customWidth="1"/>
-    <col min="12" max="12" width="28.33203125" customWidth="1"/>
+    <col min="12" max="12" width="29" customWidth="1"/>
     <col min="13" max="13" width="12.5546875" customWidth="1"/>
     <col min="14" max="14" width="27.44140625" customWidth="1"/>
     <col min="15" max="15" width="25.44140625" customWidth="1"/>
@@ -1333,26 +1326,26 @@
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q1" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="Q1" s="30" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1386,7 +1379,7 @@
       <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="18" t="s">
         <v>121</v>
       </c>
       <c r="L2" s="14" t="s">
@@ -1439,7 +1432,7 @@
       <c r="J3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="18" t="s">
         <v>131</v>
       </c>
       <c r="L3" s="14" t="s">
@@ -1492,7 +1485,7 @@
       <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="18" t="s">
         <v>122</v>
       </c>
       <c r="L4" s="14" t="s">
@@ -1545,7 +1538,7 @@
       <c r="J5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="18" t="s">
         <v>134</v>
       </c>
       <c r="L5" s="14" t="s">
@@ -1598,7 +1591,7 @@
       <c r="J6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="18" t="s">
         <v>135</v>
       </c>
       <c r="L6" s="14" t="s">
@@ -1651,7 +1644,7 @@
       <c r="J7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="18" t="s">
         <v>137</v>
       </c>
       <c r="L7" s="14" t="s">
@@ -1704,7 +1697,7 @@
       <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="18" t="s">
         <v>139</v>
       </c>
       <c r="L8" s="14" t="s">
@@ -1757,7 +1750,7 @@
       <c r="J9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="18" t="s">
         <v>141</v>
       </c>
       <c r="L9" s="14" t="s">
@@ -1810,7 +1803,7 @@
       <c r="J10" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="18" t="s">
         <v>143</v>
       </c>
       <c r="L10" s="14" t="s">
@@ -1863,7 +1856,7 @@
       <c r="J11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="18" t="s">
         <v>126</v>
       </c>
       <c r="L11" s="14" t="s">
@@ -1916,7 +1909,7 @@
       <c r="J12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="18" t="s">
         <v>145</v>
       </c>
       <c r="L12" s="14" t="s">
@@ -1969,7 +1962,7 @@
       <c r="J13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="18" t="s">
         <v>147</v>
       </c>
       <c r="L13" s="14" t="s">
@@ -2022,7 +2015,7 @@
       <c r="J14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="K14" s="18" t="s">
         <v>128</v>
       </c>
       <c r="L14" s="14" t="s">
@@ -2075,7 +2068,7 @@
       <c r="J15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="18" t="s">
         <v>58</v>
       </c>
       <c r="L15" s="14" t="s">
@@ -2128,7 +2121,7 @@
       <c r="J16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="18" t="s">
         <v>150</v>
       </c>
       <c r="L16" s="14" t="s">
@@ -2181,7 +2174,7 @@
       <c r="J17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="27" t="s">
+      <c r="K17" s="18" t="s">
         <v>151</v>
       </c>
       <c r="L17" s="14" t="s">
@@ -2234,7 +2227,7 @@
       <c r="J18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="27" t="s">
+      <c r="K18" s="18" t="s">
         <v>152</v>
       </c>
       <c r="L18" s="14" t="s">
@@ -2287,7 +2280,7 @@
       <c r="J19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="27" t="s">
+      <c r="K19" s="18" t="s">
         <v>153</v>
       </c>
       <c r="L19" s="14" t="s">
@@ -2310,96 +2303,90 @@
       </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="L20" s="28"/>
-      <c r="M20" s="29"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="15"/>
     </row>
-    <row r="21" spans="1:17">
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-    </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="20"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="28"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="2">
         <v>1</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
       <c r="L23" s="16"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="2">
         <v>2</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
       <c r="L24" s="16"/>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="2">
         <v>3</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
       <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="2">
         <v>4</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
       <c r="L26" s="16"/>
     </row>
   </sheetData>
@@ -3215,86 +3202,86 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="2">
         <v>1</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
       <c r="L23" s="16"/>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2">
         <v>2</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
       <c r="L24" s="16"/>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2">
         <v>3</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
       <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="2">
         <v>4</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
       <c r="L26" s="16"/>
     </row>
   </sheetData>
@@ -3311,20 +3298,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB60AA9-9903-422B-A5D3-D91275F59C34}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DC6A67-9716-471F-B242-870F8D2F0ED7}">
   <dimension ref="A1:D34"/>
   <sheetViews>
@@ -3379,7 +3352,7 @@
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -3388,30 +3361,30 @@
       <c r="C4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="24"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="24"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="26"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -3420,173 +3393,173 @@
       <c r="C7" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="24" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="24"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="24"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="12" t="s">
         <v>81</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="24"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="24"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="12" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="24"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="24"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="24"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="12" t="s">
         <v>108</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="24"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="22"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="24"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="24"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="12" t="s">
         <v>106</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="24"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="12" t="s">
         <v>110</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="24"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="12" t="s">
         <v>112</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="24"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="24"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="12" t="s">
         <v>113</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="25"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="24"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="23"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="27" t="s">
         <v>77</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="11"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="24"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="24"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="23"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="10" t="s">
@@ -3599,7 +3572,7 @@
       <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="27" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -3608,87 +3581,87 @@
       <c r="C26" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D26" s="21"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="24"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="24"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="12" t="s">
         <v>98</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="24"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="22"/>
+      <c r="D29" s="25"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="24"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="25"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="24"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="25"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="24"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="25"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="24"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="12" t="s">
         <v>95</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="22"/>
+      <c r="D33" s="25"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="24"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="12" t="s">
         <v>82</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="23"/>
+      <c r="D34" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>